<commit_message>
Completed the student data fetching andgenerating final company sheet with all student details.
</commit_message>
<xml_diff>
--- a/Data/GRnumbers.xlsx
+++ b/Data/GRnumbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\EXCELFILES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\UiPath\ExcelAutomationDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B69747-1145-48EF-82AD-887E47263A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CCDBAE-C1B8-4B61-8733-5D1C6B72D8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="19572" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,47 +411,157 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>21810210</v>
+        <v>21810496</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>21810183</v>
+        <v>21810685</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>21810238</v>
+        <v>21810293</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>21920154</v>
+        <v>21920031</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>21810271</v>
+        <v>21810244</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>21810372</v>
+        <v>21810277</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>21810938</v>
+        <v>21810275</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>21810751</v>
+        <v>21810417</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>21810866</v>
+        <v>21810282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>21810878</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>21920063</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>21810308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>21920157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>21810099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>21810149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21810427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>21810824</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>21810251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>21810565</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>21810827</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>21810169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>21810535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>21810715</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>21810483</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>21810228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>21810364</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>21810339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>21810590</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>21810062</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>21810261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>21810703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>